<commit_message>
Fixed make scens and make optims
</commit_message>
<xml_diff>
--- a/applications/master/data/national/default_options.xlsx
+++ b/applications/master/data/national/default_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2DA30B61-72A3-494B-8863-5EE692052475}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1FC49247-B886-1C43-BD88-5AE2831CDE51}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="76">
   <si>
     <t>Coverage</t>
   </si>
@@ -882,8 +882,8 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1115,13 +1115,17 @@
       <c r="A37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
@@ -1293,8 +1297,8 @@
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A21" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2156,7 +2160,9 @@
         <v>0</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
+      <c r="D42" s="8">
+        <v>0.95</v>
+      </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -2175,7 +2181,9 @@
         <v>0</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="8"/>
+      <c r="D43" s="8">
+        <v>0.95</v>
+      </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -2968,8 +2976,8 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScale="174" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed import statements, moved some functions to utils
</commit_message>
<xml_diff>
--- a/applications/master/data/national/default_options.xlsx
+++ b/applications/master/data/national/default_options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1FC49247-B886-1C43-BD88-5AE2831CDE51}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A33DA1DC-A454-DE42-98CB-DF90493D1918}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="4" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs to include" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="74">
   <si>
     <t>Coverage</t>
   </si>
@@ -262,9 +262,6 @@
     <t>thrive</t>
   </si>
   <si>
-    <t>1,2</t>
-  </si>
-  <si>
     <t>start year</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
   </si>
   <si>
     <t>outcomes</t>
-  </si>
-  <si>
-    <t>optim type</t>
   </si>
   <si>
     <t>false</t>
@@ -335,7 +329,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,12 +345,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -412,9 +400,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -882,7 +867,7 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -1249,19 +1234,19 @@
         <v>59</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2974,80 +2959,62 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="10">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
         <v>2017</v>
       </c>
-      <c r="E2" s="10">
+      <c r="B2" s="10">
         <v>2025</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>67</v>
       </c>
+      <c r="D2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
       <c r="G2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1000000</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved iycf cost calc to spreadsheet
</commit_message>
<xml_diff>
--- a/applications/master/data/national/default_options.xlsx
+++ b/applications/master/data/national/default_options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A399B1EC-E1FE-114A-8018-B5CEFAB2C353}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8CA9B250-9F4F-9E4F-9876-F7F9C63D8509}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs to include" sheetId="3" r:id="rId1"/>
@@ -846,8 +846,8 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1202,7 +1202,7 @@
   </sheetPr>
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+    <sheetView zoomScale="94" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Results classes to process scenarios and optimisations
</commit_message>
<xml_diff>
--- a/applications/master/data/national/default_options.xlsx
+++ b/applications/master/data/national/default_options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8CA9B250-9F4F-9E4F-9876-F7F9C63D8509}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1D924131-2131-0A48-9334-F65D53622BE5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs to include" sheetId="3" r:id="rId1"/>
@@ -261,7 +261,7 @@
     <t>filter programs</t>
   </si>
   <si>
-    <t>0,1</t>
+    <t>0,1,2</t>
   </si>
 </sst>
 </file>
@@ -846,7 +846,7 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -3743,7 +3743,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed treatment of MAM, added extension to treatment of SAM
</commit_message>
<xml_diff>
--- a/applications/master/data/national/default_options.xlsx
+++ b/applications/master/data/national/default_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C9A968BA-742B-5E4F-9F00-857BE6632D93}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{53FB4F29-1DEE-3C4F-AA8D-65ABD502E55C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31440" yWindow="-20760" windowWidth="27360" windowHeight="20240" activeTab="2" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="50">
   <si>
     <t>Coverage</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Treatment of SAM</t>
   </si>
   <si>
-    <t>Treatment of MAM</t>
-  </si>
-  <si>
     <t>Micronutrient powders</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
   </si>
   <si>
     <t>filter programs</t>
-  </si>
-  <si>
-    <t>0,1,2</t>
   </si>
   <si>
     <t>IFAS: community</t>
@@ -371,6 +365,7 @@
       <sheetName val="Time trends"/>
       <sheetName val="Fertility risks"/>
       <sheetName val="IYCF packages"/>
+      <sheetName val="Treatment of SAM"/>
       <sheetName val="Programs cost and coverage"/>
       <sheetName val="IYCF cost"/>
       <sheetName val="Program dependencies"/>
@@ -442,8 +437,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="10">
           <cell r="C10">
@@ -480,17 +475,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -796,10 +792,10 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -814,96 +810,96 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4"/>
     </row>
@@ -927,31 +923,31 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>5</v>
@@ -959,25 +955,25 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>5</v>
@@ -985,7 +981,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>5</v>
@@ -993,7 +989,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>5</v>
@@ -1001,7 +997,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>5</v>
@@ -1009,7 +1005,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>5</v>
@@ -1017,7 +1013,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>5</v>
@@ -1025,7 +1021,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>5</v>
@@ -1033,7 +1029,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>5</v>
@@ -1041,23 +1037,15 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:B37">
-    <sortCondition ref="A2:A37"/>
+  <sortState ref="A2:B36">
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1069,10 +1057,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1122,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1156,7 +1144,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -1178,7 +1166,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -1200,7 +1188,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>0</v>
@@ -1222,7 +1210,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>0</v>
@@ -1244,7 +1232,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
@@ -1266,7 +1254,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>0</v>
@@ -1288,7 +1276,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>0</v>
@@ -1310,7 +1298,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>
@@ -1332,7 +1320,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>0</v>
@@ -1354,7 +1342,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>0</v>
@@ -1376,7 +1364,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>0</v>
@@ -1398,7 +1386,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
@@ -1420,7 +1408,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>0</v>
@@ -1442,7 +1430,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>0</v>
@@ -1530,7 +1518,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>0</v>
@@ -1552,7 +1540,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>0</v>
@@ -1574,7 +1562,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>0</v>
@@ -1596,7 +1584,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>0</v>
@@ -1618,7 +1606,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>0</v>
@@ -1642,7 +1630,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>0</v>
@@ -1664,7 +1652,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>0</v>
@@ -1686,7 +1674,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>0</v>
@@ -1708,7 +1696,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>0</v>
@@ -1732,7 +1720,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>0</v>
@@ -1756,7 +1744,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>0</v>
@@ -1780,7 +1768,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>0</v>
@@ -1804,7 +1792,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>0</v>
@@ -1828,7 +1816,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>0</v>
@@ -1852,7 +1840,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>0</v>
@@ -1876,7 +1864,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>0</v>
@@ -1900,7 +1888,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>0</v>
@@ -1923,46 +1911,22 @@
       <c r="P36" s="13"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:P37">
-    <sortCondition ref="A2:A37"/>
+  <sortState ref="A2:P36">
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1974,10 +1938,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2048,7 +2012,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -2070,7 +2034,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -2092,7 +2056,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -2114,7 +2078,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>1</v>
@@ -2136,7 +2100,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>1</v>
@@ -2158,7 +2122,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>1</v>
@@ -2180,7 +2144,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>1</v>
@@ -2202,7 +2166,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>1</v>
@@ -2224,7 +2188,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>1</v>
@@ -2246,7 +2210,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>1</v>
@@ -2268,7 +2232,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>1</v>
@@ -2290,7 +2254,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>1</v>
@@ -2312,7 +2276,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>1</v>
@@ -2334,7 +2298,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>1</v>
@@ -2356,7 +2320,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>1</v>
@@ -2444,7 +2408,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>1</v>
@@ -2466,7 +2430,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>1</v>
@@ -2488,7 +2452,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>1</v>
@@ -2510,7 +2474,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>1</v>
@@ -2532,7 +2496,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>1</v>
@@ -2554,7 +2518,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>1</v>
@@ -2576,7 +2540,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>1</v>
@@ -2598,7 +2562,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>1</v>
@@ -2620,7 +2584,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>1</v>
@@ -2642,7 +2606,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>1</v>
@@ -2664,7 +2628,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>1</v>
@@ -2686,7 +2650,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>1</v>
@@ -2708,7 +2672,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>1</v>
@@ -2730,7 +2694,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>1</v>
@@ -2752,7 +2716,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>1</v>
@@ -2774,7 +2738,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>1</v>
@@ -2796,7 +2760,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>1</v>
@@ -2817,40 +2781,18 @@
       <c r="P36" s="13"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2866,7 +2808,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2877,25 +2819,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2906,19 +2848,19 @@
         <v>2025</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="11">
         <v>1000000</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>47</v>
+      <c r="F2" s="8">
+        <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added modalities for IFAS for PW,
</commit_message>
<xml_diff>
--- a/applications/master/data/national/default_options.xlsx
+++ b/applications/master/data/national/default_options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{53FB4F29-1DEE-3C4F-AA8D-65ABD502E55C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CEC91D40-EC57-974C-843A-A406205B55D0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31440" yWindow="-20760" windowWidth="27360" windowHeight="20240" activeTab="2" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
+    <workbookView xWindow="-28620" yWindow="-20940" windowWidth="27360" windowHeight="20240" activeTab="2" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs to include" sheetId="3" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="51">
   <si>
     <t>Coverage</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Iron and iodine fortification of salt</t>
   </si>
   <si>
-    <t>Iron and folic acid supplementation for pregnant women</t>
-  </si>
-  <si>
     <t>IPTp</t>
   </si>
   <si>
@@ -195,16 +192,22 @@
     <t>filter programs</t>
   </si>
   <si>
-    <t>IFAS: community</t>
-  </si>
-  <si>
-    <t>IFAS: hospital</t>
-  </si>
-  <si>
-    <t>IFAS: retailer</t>
-  </si>
-  <si>
-    <t>IFAS: school</t>
+    <t>IFAS for pregnant women (community)</t>
+  </si>
+  <si>
+    <t>IFAS (community)</t>
+  </si>
+  <si>
+    <t>IFAS (hospital)</t>
+  </si>
+  <si>
+    <t>IFAS (retailer)</t>
+  </si>
+  <si>
+    <t>IFAS (school)</t>
+  </si>
+  <si>
+    <t>IFAS for pregnant women (hospital)</t>
   </si>
 </sst>
 </file>
@@ -437,8 +440,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="10">
           <cell r="C10">
@@ -475,18 +478,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -792,10 +795,10 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -810,54 +813,54 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4"/>
     </row>
@@ -887,101 +890,99 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>5</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>5</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>5</v>
@@ -989,7 +990,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>5</v>
@@ -997,7 +998,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>5</v>
@@ -1005,7 +1006,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>5</v>
@@ -1013,7 +1014,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>5</v>
@@ -1021,7 +1022,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>5</v>
@@ -1029,7 +1030,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>5</v>
@@ -1037,15 +1038,23 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B36">
-    <sortCondition ref="A2:A36"/>
+  <sortState ref="A2:B37">
+    <sortCondition ref="A2:A37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1057,10 +1066,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1131,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1144,7 +1153,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -1166,7 +1175,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -1188,7 +1197,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>0</v>
@@ -1210,7 +1219,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>0</v>
@@ -1232,7 +1241,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
@@ -1254,7 +1263,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>0</v>
@@ -1276,7 +1285,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>0</v>
@@ -1386,7 +1395,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
@@ -1408,7 +1417,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>0</v>
@@ -1430,7 +1439,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>0</v>
@@ -1452,7 +1461,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>0</v>
@@ -1474,7 +1483,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>0</v>
@@ -1496,7 +1505,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>0</v>
@@ -1518,7 +1527,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>0</v>
@@ -1540,7 +1549,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>0</v>
@@ -1562,7 +1571,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>0</v>
@@ -1584,7 +1593,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>0</v>
@@ -1606,15 +1615,13 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="13">
-        <v>0.95</v>
-      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -1630,10 +1637,922 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:P37">
+    <sortCondition ref="A2:A37"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8FFD43-0A0F-4D4C-8EFD-D178D6D096FB}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:X38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="2">
+        <v>2020</v>
+      </c>
+      <c r="G1" s="2">
+        <v>2021</v>
+      </c>
+      <c r="H1" s="2">
+        <v>2022</v>
+      </c>
+      <c r="I1" s="2">
+        <v>2023</v>
+      </c>
+      <c r="J1" s="2">
+        <v>2024</v>
+      </c>
+      <c r="K1" s="2">
+        <v>2025</v>
+      </c>
+      <c r="L1" s="2">
+        <v>2026</v>
+      </c>
+      <c r="M1" s="2">
+        <v>2027</v>
+      </c>
+      <c r="N1" s="2">
+        <v>2028</v>
+      </c>
+      <c r="O1" s="2">
+        <v>2029</v>
+      </c>
+      <c r="P1" s="2">
+        <v>2030</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="B25" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -1652,10 +2571,10 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -1674,10 +2593,10 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1696,895 +2615,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-    </row>
-  </sheetData>
-  <sortState ref="A2:P36">
-    <sortCondition ref="A2:A36"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8FFD43-0A0F-4D4C-8EFD-D178D6D096FB}">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:X37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="56.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
-    <col min="3" max="4" width="10.83203125" style="1"/>
-    <col min="17" max="17" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2">
-        <v>2017</v>
-      </c>
-      <c r="D1" s="2">
-        <v>2018</v>
-      </c>
-      <c r="E1" s="2">
-        <v>2019</v>
-      </c>
-      <c r="F1" s="2">
-        <v>2020</v>
-      </c>
-      <c r="G1" s="2">
-        <v>2021</v>
-      </c>
-      <c r="H1" s="2">
-        <v>2022</v>
-      </c>
-      <c r="I1" s="2">
-        <v>2023</v>
-      </c>
-      <c r="J1" s="2">
-        <v>2024</v>
-      </c>
-      <c r="K1" s="2">
-        <v>2025</v>
-      </c>
-      <c r="L1" s="2">
-        <v>2026</v>
-      </c>
-      <c r="M1" s="2">
-        <v>2027</v>
-      </c>
-      <c r="N1" s="2">
-        <v>2028</v>
-      </c>
-      <c r="O1" s="2">
-        <v>2029</v>
-      </c>
-      <c r="P1" s="2">
-        <v>2030</v>
-      </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>1</v>
@@ -2606,7 +2637,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>1</v>
@@ -2628,7 +2659,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>1</v>
@@ -2650,7 +2681,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>1</v>
@@ -2672,7 +2703,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>1</v>
@@ -2694,7 +2725,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>1</v>
@@ -2716,7 +2747,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>1</v>
@@ -2738,7 +2769,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>1</v>
@@ -2760,7 +2791,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>1</v>
@@ -2781,20 +2812,45 @@
       <c r="P36" s="13"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
+      <c r="A37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
     </row>
   </sheetData>
+  <sortState ref="A2:P37">
+    <sortCondition ref="A2:A37"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2819,25 +2875,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2848,10 +2904,10 @@
         <v>2025</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="11">
         <v>1000000</v>
@@ -2860,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>